<commit_message>
categories and product categories tables created
</commit_message>
<xml_diff>
--- a/docs/Products.xlsx
+++ b/docs/Products.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Prds" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="PSQL" sheetId="4" r:id="rId5"/>
     <sheet name="PPHP" sheetId="6" r:id="rId6"/>
     <sheet name="CPHP" sheetId="8" r:id="rId7"/>
+    <sheet name="PCPHP" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1003,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4822,10 +4823,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D173"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6500,11 +6501,11 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B105" t="str">
         <f>VLOOKUP(A105,Prds!$A$3:$G$198,2)</f>
-        <v>251 outdoor speakers</v>
+        <v>SoundTouch outdoor wireless system with 251 speakers</v>
       </c>
       <c r="C105">
         <v>15</v>
@@ -6516,11 +6517,11 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B106" t="str">
         <f>VLOOKUP(A106,Prds!$A$3:$G$198,2)</f>
-        <v>SoundTouch outdoor wireless system with 251 speakers</v>
+        <v>201 bookshelf speakers</v>
       </c>
       <c r="C106">
         <v>15</v>
@@ -6532,11 +6533,11 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B107" t="str">
         <f>VLOOKUP(A107,Prds!$A$3:$G$198,2)</f>
-        <v>201 bookshelf speakers</v>
+        <v>891 in-wall speakers</v>
       </c>
       <c r="C107">
         <v>15</v>
@@ -6548,11 +6549,11 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B108" t="str">
         <f>VLOOKUP(A108,Prds!$A$3:$G$198,2)</f>
-        <v>891 in-wall speakers</v>
+        <v>591 in-ceiling speakers</v>
       </c>
       <c r="C108">
         <v>15</v>
@@ -6564,11 +6565,11 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B109" t="str">
         <f>VLOOKUP(A109,Prds!$A$3:$G$198,2)</f>
-        <v>591 in-ceiling speakers</v>
+        <v>691 in-wall speakers</v>
       </c>
       <c r="C109">
         <v>15</v>
@@ -6580,27 +6581,27 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B110" t="str">
         <f>VLOOKUP(A110,Prds!$A$3:$G$198,2)</f>
-        <v>691 in-wall speakers</v>
+        <v>Companion 2 computer speakers</v>
       </c>
       <c r="C110">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D110" t="str">
         <f>VLOOKUP(C110,Cats!$A$3:$I$20,2)</f>
-        <v>Stereo</v>
+        <v>Computer</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B111" t="str">
         <f>VLOOKUP(A111,Prds!$A$3:$G$198,2)</f>
-        <v>Companion 2 computer speakers</v>
+        <v>Companion 20 computer speakers</v>
       </c>
       <c r="C111">
         <v>16</v>
@@ -6612,27 +6613,27 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B112" t="str">
         <f>VLOOKUP(A112,Prds!$A$3:$G$198,2)</f>
-        <v>Companion 20 computer speakers</v>
+        <v>S1 Pro system</v>
       </c>
       <c r="C112">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D112" t="str">
         <f>VLOOKUP(C112,Cats!$A$3:$I$20,2)</f>
-        <v>Computer</v>
+        <v>Portable PA</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B113" t="str">
         <f>VLOOKUP(A113,Prds!$A$3:$G$198,2)</f>
-        <v>S1 Pro system</v>
+        <v>L1 Compact system</v>
       </c>
       <c r="C113">
         <v>17</v>
@@ -6644,11 +6645,11 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B114" t="str">
         <f>VLOOKUP(A114,Prds!$A$3:$G$198,2)</f>
-        <v>L1 Compact system</v>
+        <v>F1 Model 812 loudspeaker with F1 Subwoofer</v>
       </c>
       <c r="C114">
         <v>17</v>
@@ -6660,11 +6661,11 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B115" t="str">
         <f>VLOOKUP(A115,Prds!$A$3:$G$198,2)</f>
-        <v>F1 Model 812 loudspeaker with F1 Subwoofer</v>
+        <v>F1 Model 812 Flexible Array loudspeaker</v>
       </c>
       <c r="C115">
         <v>17</v>
@@ -6676,11 +6677,11 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B116" t="str">
         <f>VLOOKUP(A116,Prds!$A$3:$G$198,2)</f>
-        <v>F1 Model 812 Flexible Array loudspeaker</v>
+        <v>L1 II system/B2 bass</v>
       </c>
       <c r="C116">
         <v>17</v>
@@ -6692,11 +6693,11 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B117" t="str">
         <f>VLOOKUP(A117,Prds!$A$3:$G$198,2)</f>
-        <v>L1 II system/B2 bass</v>
+        <v>L1 Compact Wireless package</v>
       </c>
       <c r="C117">
         <v>17</v>
@@ -6708,11 +6709,11 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B118" t="str">
         <f>VLOOKUP(A118,Prds!$A$3:$G$198,2)</f>
-        <v>L1 Compact Wireless package</v>
+        <v>T4S ToneMatch mixer</v>
       </c>
       <c r="C118">
         <v>17</v>
@@ -6724,11 +6725,11 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B119" t="str">
         <f>VLOOKUP(A119,Prds!$A$3:$G$198,2)</f>
-        <v>T4S ToneMatch mixer</v>
+        <v>T8S ToneMatch mixer</v>
       </c>
       <c r="C119">
         <v>17</v>
@@ -6740,11 +6741,11 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B120" t="str">
         <f>VLOOKUP(A120,Prds!$A$3:$G$198,2)</f>
-        <v>T8S ToneMatch mixer</v>
+        <v>F1 Subwoofer</v>
       </c>
       <c r="C120">
         <v>17</v>
@@ -6756,11 +6757,11 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B121" t="str">
         <f>VLOOKUP(A121,Prds!$A$3:$G$198,2)</f>
-        <v>F1 Subwoofer</v>
+        <v>L1 1S system/B2 bass</v>
       </c>
       <c r="C121">
         <v>17</v>
@@ -6772,11 +6773,11 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B122" t="str">
         <f>VLOOKUP(A122,Prds!$A$3:$G$198,2)</f>
-        <v>L1 1S system/B2 bass</v>
+        <v>L1 1S system/B1 bass</v>
       </c>
       <c r="C122">
         <v>17</v>
@@ -6788,11 +6789,11 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B123" t="str">
         <f>VLOOKUP(A123,Prds!$A$3:$G$198,2)</f>
-        <v>L1 1S system/B1 bass</v>
+        <v>L1 II system/B1 bass</v>
       </c>
       <c r="C123">
         <v>17</v>
@@ -6804,11 +6805,11 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B124" t="str">
         <f>VLOOKUP(A124,Prds!$A$3:$G$198,2)</f>
-        <v>L1 II system/B1 bass</v>
+        <v>Two F1 Model 812 loudspeakers with F1 Subwoofer</v>
       </c>
       <c r="C124">
         <v>17</v>
@@ -6820,27 +6821,27 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="B125" t="str">
         <f>VLOOKUP(A125,Prds!$A$3:$G$198,2)</f>
-        <v>Two F1 Model 812 loudspeakers with F1 Subwoofer</v>
+        <v>Bose Surround Speakers</v>
       </c>
       <c r="C125">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D125" t="str">
         <f>VLOOKUP(C125,Cats!$A$3:$I$20,2)</f>
-        <v>Portable PA</v>
+        <v>Speaker Accesories</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B126" t="str">
         <f>VLOOKUP(A126,Prds!$A$3:$G$198,2)</f>
-        <v>Bose Surround Speakers</v>
+        <v>Bose Bass Module 700</v>
       </c>
       <c r="C126">
         <v>18</v>
@@ -6852,11 +6853,11 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B127" t="str">
         <f>VLOOKUP(A127,Prds!$A$3:$G$198,2)</f>
-        <v>Bose Bass Module 700</v>
+        <v>Bose Bass Module 500</v>
       </c>
       <c r="C127">
         <v>18</v>
@@ -6868,11 +6869,11 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="B128" t="str">
         <f>VLOOKUP(A128,Prds!$A$3:$G$198,2)</f>
-        <v>Bose Bass Module 500</v>
+        <v>SoundLink Revolve charging cradle</v>
       </c>
       <c r="C128">
         <v>18</v>
@@ -6884,11 +6885,11 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B129" t="str">
         <f>VLOOKUP(A129,Prds!$A$3:$G$198,2)</f>
-        <v>SoundLink Revolve charging cradle</v>
+        <v>Bose Soundbar Wall Bracket</v>
       </c>
       <c r="C129">
         <v>18</v>
@@ -6900,11 +6901,11 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B130" t="str">
         <f>VLOOKUP(A130,Prds!$A$3:$G$198,2)</f>
-        <v>Bose Soundbar Wall Bracket</v>
+        <v>Bose Soundbar Universal Remote</v>
       </c>
       <c r="C130">
         <v>18</v>
@@ -6916,11 +6917,11 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B131" t="str">
         <f>VLOOKUP(A131,Prds!$A$3:$G$198,2)</f>
-        <v>Bose Soundbar Universal Remote</v>
+        <v>SoundXtra TV stand for SoundTouch 300</v>
       </c>
       <c r="C131">
         <v>18</v>
@@ -6932,11 +6933,11 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B132" t="str">
         <f>VLOOKUP(A132,Prds!$A$3:$G$198,2)</f>
-        <v>SoundXtra TV stand for SoundTouch 300</v>
+        <v>S1 Pro Slip Cover</v>
       </c>
       <c r="C132">
         <v>18</v>
@@ -6948,11 +6949,11 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B133" t="str">
         <f>VLOOKUP(A133,Prds!$A$3:$G$198,2)</f>
-        <v>S1 Pro Slip Cover</v>
+        <v>S1 Pro Backpack</v>
       </c>
       <c r="C133">
         <v>18</v>
@@ -6964,11 +6965,11 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B134" t="str">
         <f>VLOOKUP(A134,Prds!$A$3:$G$198,2)</f>
-        <v>S1 Pro Backpack</v>
+        <v>SoundXtra floor stand for SoundTouch 20</v>
       </c>
       <c r="C134">
         <v>18</v>
@@ -6980,11 +6981,11 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B135" t="str">
         <f>VLOOKUP(A135,Prds!$A$3:$G$198,2)</f>
-        <v>SoundXtra floor stand for SoundTouch 20</v>
+        <v>Wave FM antenna</v>
       </c>
       <c r="C135">
         <v>18</v>
@@ -6996,11 +6997,11 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B136" t="str">
         <f>VLOOKUP(A136,Prds!$A$3:$G$198,2)</f>
-        <v>Wave FM antenna</v>
+        <v>RC-PWS III universal remote</v>
       </c>
       <c r="C136">
         <v>18</v>
@@ -7012,11 +7013,11 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B137" t="str">
         <f>VLOOKUP(A137,Prds!$A$3:$G$198,2)</f>
-        <v>RC-PWS III universal remote</v>
+        <v>UB-20 II wall/ceiling bracket</v>
       </c>
       <c r="C137">
         <v>18</v>
@@ -7028,11 +7029,11 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B138" t="str">
         <f>VLOOKUP(A138,Prds!$A$3:$G$198,2)</f>
-        <v>UB-20 II wall/ceiling bracket</v>
+        <v>UFS-20 II floorstands</v>
       </c>
       <c r="C138">
         <v>18</v>
@@ -7044,11 +7045,11 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B139" t="str">
         <f>VLOOKUP(A139,Prds!$A$3:$G$198,2)</f>
-        <v>UFS-20 II floorstands</v>
+        <v>SoundWear Companion cover</v>
       </c>
       <c r="C139">
         <v>18</v>
@@ -7060,11 +7061,11 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B140" t="str">
         <f>VLOOKUP(A140,Prds!$A$3:$G$198,2)</f>
-        <v>SoundWear Companion cover</v>
+        <v>T4S ToneMatch mixer</v>
       </c>
       <c r="C140">
         <v>18</v>
@@ -7076,11 +7077,11 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="B141" t="str">
         <f>VLOOKUP(A141,Prds!$A$3:$G$198,2)</f>
-        <v>T4S ToneMatch mixer</v>
+        <v>Speaker wire adapter kot</v>
       </c>
       <c r="C141">
         <v>18</v>
@@ -7092,11 +7093,11 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B142" t="str">
         <f>VLOOKUP(A142,Prds!$A$3:$G$198,2)</f>
-        <v>Speaker wire adapter kot</v>
+        <v>B1 bass module</v>
       </c>
       <c r="C142">
         <v>18</v>
@@ -7108,11 +7109,11 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B143" t="str">
         <f>VLOOKUP(A143,Prds!$A$3:$G$198,2)</f>
-        <v>B1 bass module</v>
+        <v>T8S ToneMatch mixer</v>
       </c>
       <c r="C143">
         <v>18</v>
@@ -7124,11 +7125,11 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B144" t="str">
         <f>VLOOKUP(A144,Prds!$A$3:$G$198,2)</f>
-        <v>T8S ToneMatch mixer</v>
+        <v>SlideConnect wall bracket</v>
       </c>
       <c r="C144">
         <v>18</v>
@@ -7140,11 +7141,11 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B145" t="str">
         <f>VLOOKUP(A145,Prds!$A$3:$G$198,2)</f>
-        <v>SlideConnect wall bracket</v>
+        <v>WB-300 wall bracket</v>
       </c>
       <c r="C145">
         <v>18</v>
@@ -7156,11 +7157,11 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B146" t="str">
         <f>VLOOKUP(A146,Prds!$A$3:$G$198,2)</f>
-        <v>WB-300 wall bracket</v>
+        <v>WB-120 wall-mount kit</v>
       </c>
       <c r="C146">
         <v>18</v>
@@ -7172,11 +7173,11 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="B147" t="str">
         <f>VLOOKUP(A147,Prds!$A$3:$G$198,2)</f>
-        <v>WB-120 wall-mount kit</v>
+        <v>F1 Subwoofer</v>
       </c>
       <c r="C147">
         <v>18</v>
@@ -7188,11 +7189,11 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="B148" t="str">
         <f>VLOOKUP(A148,Prds!$A$3:$G$198,2)</f>
-        <v>F1 Subwoofer</v>
+        <v>L1 Compact microphone accessory pack</v>
       </c>
       <c r="C148">
         <v>18</v>
@@ -7204,11 +7205,11 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B149" t="str">
         <f>VLOOKUP(A149,Prds!$A$3:$G$198,2)</f>
-        <v>L1 Compact microphone accessory pack</v>
+        <v>SoundLink Mini travel bag</v>
       </c>
       <c r="C149">
         <v>18</v>
@@ -7220,11 +7221,11 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B150" t="str">
         <f>VLOOKUP(A150,Prds!$A$3:$G$198,2)</f>
-        <v>SoundLink Mini travel bag</v>
+        <v>UTS-20 II table stand</v>
       </c>
       <c r="C150">
         <v>18</v>
@@ -7236,11 +7237,11 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B151" t="str">
         <f>VLOOKUP(A151,Prds!$A$3:$G$198,2)</f>
-        <v>UTS-20 II table stand</v>
+        <v>CineMate speaker wire adapter kit</v>
       </c>
       <c r="C151">
         <v>18</v>
@@ -7252,11 +7253,11 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B152" t="str">
         <f>VLOOKUP(A152,Prds!$A$3:$G$198,2)</f>
-        <v>CineMate speaker wire adapter kit</v>
+        <v>B1/B2 4-pin cable</v>
       </c>
       <c r="C152">
         <v>18</v>
@@ -7268,11 +7269,11 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B153" t="str">
         <f>VLOOKUP(A153,Prds!$A$3:$G$198,2)</f>
-        <v>B1/B2 4-pin cable</v>
+        <v>SoundXtra TV mount for SoundTouch 300</v>
       </c>
       <c r="C153">
         <v>18</v>
@@ -7284,11 +7285,11 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B154" t="str">
         <f>VLOOKUP(A154,Prds!$A$3:$G$198,2)</f>
-        <v>SoundXtra TV mount for SoundTouch 300</v>
+        <v>SoundLink speaker III cover</v>
       </c>
       <c r="C154">
         <v>18</v>
@@ -7300,11 +7301,11 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B155" t="str">
         <f>VLOOKUP(A155,Prds!$A$3:$G$198,2)</f>
-        <v>SoundLink speaker III cover</v>
+        <v>PackLite A1 power amplifier</v>
       </c>
       <c r="C155">
         <v>18</v>
@@ -7316,11 +7317,11 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B156" t="str">
         <f>VLOOKUP(A156,Prds!$A$3:$G$198,2)</f>
-        <v>PackLite A1 power amplifier</v>
+        <v>WB-3 bookshelf speaker wall brackets</v>
       </c>
       <c r="C156">
         <v>18</v>
@@ -7332,11 +7333,11 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B157" t="str">
         <f>VLOOKUP(A157,Prds!$A$3:$G$198,2)</f>
-        <v>WB-3 bookshelf speaker wall brackets</v>
+        <v>B2 bass module</v>
       </c>
       <c r="C157">
         <v>18</v>
@@ -7348,11 +7349,11 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B158" t="str">
         <f>VLOOKUP(A158,Prds!$A$3:$G$198,2)</f>
-        <v>B2 bass module</v>
+        <v>ToneMatch mixer power supply</v>
       </c>
       <c r="C158">
         <v>18</v>
@@ -7364,11 +7365,11 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B159" t="str">
         <f>VLOOKUP(A159,Prds!$A$3:$G$198,2)</f>
-        <v>ToneMatch mixer power supply</v>
+        <v>SoundLink Revolve and Soundlink Revolve+ wall adapter</v>
       </c>
       <c r="C159">
         <v>18</v>
@@ -7380,11 +7381,11 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B160" t="str">
         <f>VLOOKUP(A160,Prds!$A$3:$G$198,2)</f>
-        <v>SoundLink Revolve and Soundlink Revolve+ wall adapter</v>
+        <v>FS-01 bookshelf speaker floorstands</v>
       </c>
       <c r="C160">
         <v>18</v>
@@ -7396,11 +7397,11 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B161" t="str">
         <f>VLOOKUP(A161,Prds!$A$3:$G$198,2)</f>
-        <v>FS-01 bookshelf speaker floorstands</v>
+        <v>Home theater speaker extension cable</v>
       </c>
       <c r="C161">
         <v>18</v>
@@ -7412,11 +7413,11 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B162" t="str">
         <f>VLOOKUP(A162,Prds!$A$3:$G$198,2)</f>
-        <v>Home theater speaker extension cable</v>
+        <v>Lifestyle 600/650 home entertainment system remote control</v>
       </c>
       <c r="C162">
         <v>18</v>
@@ -7428,11 +7429,11 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B163" t="str">
         <f>VLOOKUP(A163,Prds!$A$3:$G$198,2)</f>
-        <v>Lifestyle 600/650 home entertainment system remote control</v>
+        <v>SoundTouch II remote</v>
       </c>
       <c r="C163">
         <v>18</v>
@@ -7444,11 +7445,11 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B164" t="str">
         <f>VLOOKUP(A164,Prds!$A$3:$G$198,2)</f>
-        <v>SoundTouch II remote</v>
+        <v>OmniJewel center channel wire adapter</v>
       </c>
       <c r="C164">
         <v>18</v>
@@ -7460,11 +7461,11 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B165" t="str">
         <f>VLOOKUP(A165,Prds!$A$3:$G$198,2)</f>
-        <v>OmniJewel center channel wire adapter</v>
+        <v>SoundXtra wall mount for SoundTouch 10</v>
       </c>
       <c r="C165">
         <v>18</v>
@@ -7476,11 +7477,11 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B166" t="str">
         <f>VLOOKUP(A166,Prds!$A$3:$G$198,2)</f>
-        <v>SoundXtra wall mount for SoundTouch 10</v>
+        <v>791 in-ceiling speakers II rough-in kit</v>
       </c>
       <c r="C166">
         <v>18</v>
@@ -7492,11 +7493,11 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B167" t="str">
         <f>VLOOKUP(A167,Prds!$A$3:$G$198,2)</f>
-        <v>791 in-ceiling speakers II rough-in kit</v>
+        <v>WB-135 wall mount kit</v>
       </c>
       <c r="C167">
         <v>18</v>
@@ -7508,11 +7509,11 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B168" t="str">
         <f>VLOOKUP(A168,Prds!$A$3:$G$198,2)</f>
-        <v>WB-135 wall mount kit</v>
+        <v>CineMate home theater system-Interface Module</v>
       </c>
       <c r="C168">
         <v>18</v>
@@ -7524,11 +7525,11 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B169" t="str">
         <f>VLOOKUP(A169,Prds!$A$3:$G$198,2)</f>
-        <v>CineMate home theater system-Interface Module</v>
+        <v>F1 Model 812 travel bag</v>
       </c>
       <c r="C169">
         <v>18</v>
@@ -7540,11 +7541,11 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B170" t="str">
         <f>VLOOKUP(A170,Prds!$A$3:$G$198,2)</f>
-        <v>F1 Model 812 travel bag</v>
+        <v>891 in-wall speakers rough-in kit</v>
       </c>
       <c r="C170">
         <v>18</v>
@@ -7556,11 +7557,11 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B171" t="str">
         <f>VLOOKUP(A171,Prds!$A$3:$G$198,2)</f>
-        <v>891 in-wall speakers rough-in kit</v>
+        <v>SoundXtra floor stand for SoundTouch 10</v>
       </c>
       <c r="C171">
         <v>18</v>
@@ -7572,33 +7573,17 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B172" t="str">
         <f>VLOOKUP(A172,Prds!$A$3:$G$198,2)</f>
-        <v>SoundXtra floor stand for SoundTouch 10</v>
+        <v>SoundXtra floor stand for SoundTouch 30</v>
       </c>
       <c r="C172">
         <v>18</v>
       </c>
       <c r="D172" t="str">
         <f>VLOOKUP(C172,Cats!$A$3:$I$20,2)</f>
-        <v>Speaker Accesories</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173">
-        <v>160</v>
-      </c>
-      <c r="B173" t="str">
-        <f>VLOOKUP(A173,Prds!$A$3:$G$198,2)</f>
-        <v>SoundXtra floor stand for SoundTouch 30</v>
-      </c>
-      <c r="C173">
-        <v>18</v>
-      </c>
-      <c r="D173" t="str">
-        <f>VLOOKUP(C173,Cats!$A$3:$I$20,2)</f>
         <v>Speaker Accesories</v>
       </c>
     </row>
@@ -10964,7 +10949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
@@ -11081,4 +11066,1043 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A171"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A2&amp;",'category_id'=&gt;"&amp;ProdCats!C2&amp;"],"</f>
+        <v>['product_id'=&gt;1,'category_id'=&gt;3],</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A3&amp;",'category_id'=&gt;"&amp;ProdCats!C3&amp;"],"</f>
+        <v>['product_id'=&gt;2,'category_id'=&gt;3],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A4&amp;",'category_id'=&gt;"&amp;ProdCats!C4&amp;"],"</f>
+        <v>['product_id'=&gt;3,'category_id'=&gt;3],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A5&amp;",'category_id'=&gt;"&amp;ProdCats!C5&amp;"],"</f>
+        <v>['product_id'=&gt;4,'category_id'=&gt;3],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A6&amp;",'category_id'=&gt;"&amp;ProdCats!C6&amp;"],"</f>
+        <v>['product_id'=&gt;5,'category_id'=&gt;3],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A7&amp;",'category_id'=&gt;"&amp;ProdCats!C7&amp;"],"</f>
+        <v>['product_id'=&gt;6,'category_id'=&gt;3],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A8&amp;",'category_id'=&gt;"&amp;ProdCats!C8&amp;"],"</f>
+        <v>['product_id'=&gt;1,'category_id'=&gt;4],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A9&amp;",'category_id'=&gt;"&amp;ProdCats!C9&amp;"],"</f>
+        <v>['product_id'=&gt;7,'category_id'=&gt;4],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A10&amp;",'category_id'=&gt;"&amp;ProdCats!C10&amp;"],"</f>
+        <v>['product_id'=&gt;8,'category_id'=&gt;4],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A11&amp;",'category_id'=&gt;"&amp;ProdCats!C11&amp;"],"</f>
+        <v>['product_id'=&gt;2,'category_id'=&gt;4],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A12&amp;",'category_id'=&gt;"&amp;ProdCats!C12&amp;"],"</f>
+        <v>['product_id'=&gt;3,'category_id'=&gt;4],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A13&amp;",'category_id'=&gt;"&amp;ProdCats!C13&amp;"],"</f>
+        <v>['product_id'=&gt;9,'category_id'=&gt;4],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A14&amp;",'category_id'=&gt;"&amp;ProdCats!C14&amp;"],"</f>
+        <v>['product_id'=&gt;4,'category_id'=&gt;4],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A15&amp;",'category_id'=&gt;"&amp;ProdCats!C15&amp;"],"</f>
+        <v>['product_id'=&gt;12,'category_id'=&gt;4],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A16&amp;",'category_id'=&gt;"&amp;ProdCats!C16&amp;"],"</f>
+        <v>['product_id'=&gt;13,'category_id'=&gt;4],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A17&amp;",'category_id'=&gt;"&amp;ProdCats!C17&amp;"],"</f>
+        <v>['product_id'=&gt;7,'category_id'=&gt;5],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A18&amp;",'category_id'=&gt;"&amp;ProdCats!C18&amp;"],"</f>
+        <v>['product_id'=&gt;8,'category_id'=&gt;5],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A19&amp;",'category_id'=&gt;"&amp;ProdCats!C19&amp;"],"</f>
+        <v>['product_id'=&gt;14,'category_id'=&gt;5],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A20&amp;",'category_id'=&gt;"&amp;ProdCats!C20&amp;"],"</f>
+        <v>['product_id'=&gt;12,'category_id'=&gt;5],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A21&amp;",'category_id'=&gt;"&amp;ProdCats!C21&amp;"],"</f>
+        <v>['product_id'=&gt;15,'category_id'=&gt;5],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A22&amp;",'category_id'=&gt;"&amp;ProdCats!C22&amp;"],"</f>
+        <v>['product_id'=&gt;10,'category_id'=&gt;6],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A23&amp;",'category_id'=&gt;"&amp;ProdCats!C23&amp;"],"</f>
+        <v>['product_id'=&gt;20,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A24&amp;",'category_id'=&gt;"&amp;ProdCats!C24&amp;"],"</f>
+        <v>['product_id'=&gt;21,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A25&amp;",'category_id'=&gt;"&amp;ProdCats!C25&amp;"],"</f>
+        <v>['product_id'=&gt;22,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A26&amp;",'category_id'=&gt;"&amp;ProdCats!C26&amp;"],"</f>
+        <v>['product_id'=&gt;23,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A27&amp;",'category_id'=&gt;"&amp;ProdCats!C27&amp;"],"</f>
+        <v>['product_id'=&gt;24,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A28&amp;",'category_id'=&gt;"&amp;ProdCats!C28&amp;"],"</f>
+        <v>['product_id'=&gt;25,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A29&amp;",'category_id'=&gt;"&amp;ProdCats!C29&amp;"],"</f>
+        <v>['product_id'=&gt;26,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A30&amp;",'category_id'=&gt;"&amp;ProdCats!C30&amp;"],"</f>
+        <v>['product_id'=&gt;27,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A31&amp;",'category_id'=&gt;"&amp;ProdCats!C31&amp;"],"</f>
+        <v>['product_id'=&gt;28,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A32&amp;",'category_id'=&gt;"&amp;ProdCats!C32&amp;"],"</f>
+        <v>['product_id'=&gt;29,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A33&amp;",'category_id'=&gt;"&amp;ProdCats!C33&amp;"],"</f>
+        <v>['product_id'=&gt;30,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A34&amp;",'category_id'=&gt;"&amp;ProdCats!C34&amp;"],"</f>
+        <v>['product_id'=&gt;31,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A35&amp;",'category_id'=&gt;"&amp;ProdCats!C35&amp;"],"</f>
+        <v>['product_id'=&gt;32,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A36&amp;",'category_id'=&gt;"&amp;ProdCats!C36&amp;"],"</f>
+        <v>['product_id'=&gt;33,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A37&amp;",'category_id'=&gt;"&amp;ProdCats!C37&amp;"],"</f>
+        <v>['product_id'=&gt;34,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A38&amp;",'category_id'=&gt;"&amp;ProdCats!C38&amp;"],"</f>
+        <v>['product_id'=&gt;35,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A39&amp;",'category_id'=&gt;"&amp;ProdCats!C39&amp;"],"</f>
+        <v>['product_id'=&gt;36,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A40&amp;",'category_id'=&gt;"&amp;ProdCats!C40&amp;"],"</f>
+        <v>['product_id'=&gt;37,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A41&amp;",'category_id'=&gt;"&amp;ProdCats!C41&amp;"],"</f>
+        <v>['product_id'=&gt;38,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A42&amp;",'category_id'=&gt;"&amp;ProdCats!C42&amp;"],"</f>
+        <v>['product_id'=&gt;39,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A43&amp;",'category_id'=&gt;"&amp;ProdCats!C43&amp;"],"</f>
+        <v>['product_id'=&gt;40,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A44&amp;",'category_id'=&gt;"&amp;ProdCats!C44&amp;"],"</f>
+        <v>['product_id'=&gt;41,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A45&amp;",'category_id'=&gt;"&amp;ProdCats!C45&amp;"],"</f>
+        <v>['product_id'=&gt;42,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A46&amp;",'category_id'=&gt;"&amp;ProdCats!C46&amp;"],"</f>
+        <v>['product_id'=&gt;43,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A47&amp;",'category_id'=&gt;"&amp;ProdCats!C47&amp;"],"</f>
+        <v>['product_id'=&gt;44,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A48&amp;",'category_id'=&gt;"&amp;ProdCats!C48&amp;"],"</f>
+        <v>['product_id'=&gt;45,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A49&amp;",'category_id'=&gt;"&amp;ProdCats!C49&amp;"],"</f>
+        <v>['product_id'=&gt;46,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A50&amp;",'category_id'=&gt;"&amp;ProdCats!C50&amp;"],"</f>
+        <v>['product_id'=&gt;47,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A51&amp;",'category_id'=&gt;"&amp;ProdCats!C51&amp;"],"</f>
+        <v>['product_id'=&gt;48,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A52&amp;",'category_id'=&gt;"&amp;ProdCats!C52&amp;"],"</f>
+        <v>['product_id'=&gt;49,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A53&amp;",'category_id'=&gt;"&amp;ProdCats!C53&amp;"],"</f>
+        <v>['product_id'=&gt;50,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A54&amp;",'category_id'=&gt;"&amp;ProdCats!C54&amp;"],"</f>
+        <v>['product_id'=&gt;51,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A55&amp;",'category_id'=&gt;"&amp;ProdCats!C55&amp;"],"</f>
+        <v>['product_id'=&gt;52,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A56&amp;",'category_id'=&gt;"&amp;ProdCats!C56&amp;"],"</f>
+        <v>['product_id'=&gt;53,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A57&amp;",'category_id'=&gt;"&amp;ProdCats!C57&amp;"],"</f>
+        <v>['product_id'=&gt;54,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A58&amp;",'category_id'=&gt;"&amp;ProdCats!C58&amp;"],"</f>
+        <v>['product_id'=&gt;55,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A59&amp;",'category_id'=&gt;"&amp;ProdCats!C59&amp;"],"</f>
+        <v>['product_id'=&gt;56,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A60&amp;",'category_id'=&gt;"&amp;ProdCats!C60&amp;"],"</f>
+        <v>['product_id'=&gt;57,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A61&amp;",'category_id'=&gt;"&amp;ProdCats!C61&amp;"],"</f>
+        <v>['product_id'=&gt;58,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A62&amp;",'category_id'=&gt;"&amp;ProdCats!C62&amp;"],"</f>
+        <v>['product_id'=&gt;59,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A63&amp;",'category_id'=&gt;"&amp;ProdCats!C63&amp;"],"</f>
+        <v>['product_id'=&gt;60,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A64&amp;",'category_id'=&gt;"&amp;ProdCats!C64&amp;"],"</f>
+        <v>['product_id'=&gt;61,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A65&amp;",'category_id'=&gt;"&amp;ProdCats!C65&amp;"],"</f>
+        <v>['product_id'=&gt;62,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A66&amp;",'category_id'=&gt;"&amp;ProdCats!C66&amp;"],"</f>
+        <v>['product_id'=&gt;63,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A67&amp;",'category_id'=&gt;"&amp;ProdCats!C67&amp;"],"</f>
+        <v>['product_id'=&gt;64,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A68&amp;",'category_id'=&gt;"&amp;ProdCats!C68&amp;"],"</f>
+        <v>['product_id'=&gt;65,'category_id'=&gt;10],</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A69&amp;",'category_id'=&gt;"&amp;ProdCats!C69&amp;"],"</f>
+        <v>['product_id'=&gt;66,'category_id'=&gt;11],</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A70&amp;",'category_id'=&gt;"&amp;ProdCats!C70&amp;"],"</f>
+        <v>['product_id'=&gt;67,'category_id'=&gt;11],</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A71&amp;",'category_id'=&gt;"&amp;ProdCats!C71&amp;"],"</f>
+        <v>['product_id'=&gt;68,'category_id'=&gt;11],</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A72&amp;",'category_id'=&gt;"&amp;ProdCats!C72&amp;"],"</f>
+        <v>['product_id'=&gt;69,'category_id'=&gt;11],</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A73&amp;",'category_id'=&gt;"&amp;ProdCats!C73&amp;"],"</f>
+        <v>['product_id'=&gt;70,'category_id'=&gt;11],</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A74&amp;",'category_id'=&gt;"&amp;ProdCats!C74&amp;"],"</f>
+        <v>['product_id'=&gt;71,'category_id'=&gt;11],</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A75&amp;",'category_id'=&gt;"&amp;ProdCats!C75&amp;"],"</f>
+        <v>['product_id'=&gt;72,'category_id'=&gt;11],</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A76&amp;",'category_id'=&gt;"&amp;ProdCats!C76&amp;"],"</f>
+        <v>['product_id'=&gt;73,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A77&amp;",'category_id'=&gt;"&amp;ProdCats!C77&amp;"],"</f>
+        <v>['product_id'=&gt;74,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A78&amp;",'category_id'=&gt;"&amp;ProdCats!C78&amp;"],"</f>
+        <v>['product_id'=&gt;75,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A79&amp;",'category_id'=&gt;"&amp;ProdCats!C79&amp;"],"</f>
+        <v>['product_id'=&gt;76,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A80&amp;",'category_id'=&gt;"&amp;ProdCats!C80&amp;"],"</f>
+        <v>['product_id'=&gt;77,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A81&amp;",'category_id'=&gt;"&amp;ProdCats!C81&amp;"],"</f>
+        <v>['product_id'=&gt;78,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A82&amp;",'category_id'=&gt;"&amp;ProdCats!C82&amp;"],"</f>
+        <v>['product_id'=&gt;79,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A83&amp;",'category_id'=&gt;"&amp;ProdCats!C83&amp;"],"</f>
+        <v>['product_id'=&gt;80,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A84&amp;",'category_id'=&gt;"&amp;ProdCats!C84&amp;"],"</f>
+        <v>['product_id'=&gt;81,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A85&amp;",'category_id'=&gt;"&amp;ProdCats!C85&amp;"],"</f>
+        <v>['product_id'=&gt;82,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A86&amp;",'category_id'=&gt;"&amp;ProdCats!C86&amp;"],"</f>
+        <v>['product_id'=&gt;83,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A87&amp;",'category_id'=&gt;"&amp;ProdCats!C87&amp;"],"</f>
+        <v>['product_id'=&gt;84,'category_id'=&gt;12],</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A88&amp;",'category_id'=&gt;"&amp;ProdCats!C88&amp;"],"</f>
+        <v>['product_id'=&gt;74,'category_id'=&gt;13],</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A89&amp;",'category_id'=&gt;"&amp;ProdCats!C89&amp;"],"</f>
+        <v>['product_id'=&gt;75,'category_id'=&gt;13],</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A90&amp;",'category_id'=&gt;"&amp;ProdCats!C90&amp;"],"</f>
+        <v>['product_id'=&gt;76,'category_id'=&gt;13],</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A91&amp;",'category_id'=&gt;"&amp;ProdCats!C91&amp;"],"</f>
+        <v>['product_id'=&gt;77,'category_id'=&gt;13],</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A92&amp;",'category_id'=&gt;"&amp;ProdCats!C92&amp;"],"</f>
+        <v>['product_id'=&gt;78,'category_id'=&gt;13],</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A93&amp;",'category_id'=&gt;"&amp;ProdCats!C93&amp;"],"</f>
+        <v>['product_id'=&gt;90,'category_id'=&gt;13],</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A94&amp;",'category_id'=&gt;"&amp;ProdCats!C94&amp;"],"</f>
+        <v>['product_id'=&gt;91,'category_id'=&gt;13],</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A95&amp;",'category_id'=&gt;"&amp;ProdCats!C95&amp;"],"</f>
+        <v>['product_id'=&gt;92,'category_id'=&gt;14],</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A96&amp;",'category_id'=&gt;"&amp;ProdCats!C96&amp;"],"</f>
+        <v>['product_id'=&gt;93,'category_id'=&gt;14],</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A97&amp;",'category_id'=&gt;"&amp;ProdCats!C97&amp;"],"</f>
+        <v>['product_id'=&gt;94,'category_id'=&gt;14],</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A98&amp;",'category_id'=&gt;"&amp;ProdCats!C98&amp;"],"</f>
+        <v>['product_id'=&gt;83,'category_id'=&gt;14],</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A99&amp;",'category_id'=&gt;"&amp;ProdCats!C99&amp;"],"</f>
+        <v>['product_id'=&gt;96,'category_id'=&gt;14],</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A100&amp;",'category_id'=&gt;"&amp;ProdCats!C100&amp;"],"</f>
+        <v>['product_id'=&gt;97,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A101&amp;",'category_id'=&gt;"&amp;ProdCats!C101&amp;"],"</f>
+        <v>['product_id'=&gt;98,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A102&amp;",'category_id'=&gt;"&amp;ProdCats!C102&amp;"],"</f>
+        <v>['product_id'=&gt;99,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A103&amp;",'category_id'=&gt;"&amp;ProdCats!C103&amp;"],"</f>
+        <v>['product_id'=&gt;100,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A104&amp;",'category_id'=&gt;"&amp;ProdCats!C104&amp;"],"</f>
+        <v>['product_id'=&gt;101,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A105&amp;",'category_id'=&gt;"&amp;ProdCats!C105&amp;"],"</f>
+        <v>['product_id'=&gt;84,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A106&amp;",'category_id'=&gt;"&amp;ProdCats!C106&amp;"],"</f>
+        <v>['product_id'=&gt;103,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A107&amp;",'category_id'=&gt;"&amp;ProdCats!C107&amp;"],"</f>
+        <v>['product_id'=&gt;104,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A108&amp;",'category_id'=&gt;"&amp;ProdCats!C108&amp;"],"</f>
+        <v>['product_id'=&gt;105,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A109&amp;",'category_id'=&gt;"&amp;ProdCats!C109&amp;"],"</f>
+        <v>['product_id'=&gt;106,'category_id'=&gt;15],</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A110&amp;",'category_id'=&gt;"&amp;ProdCats!C110&amp;"],"</f>
+        <v>['product_id'=&gt;92,'category_id'=&gt;16],</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A111&amp;",'category_id'=&gt;"&amp;ProdCats!C111&amp;"],"</f>
+        <v>['product_id'=&gt;96,'category_id'=&gt;16],</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A112&amp;",'category_id'=&gt;"&amp;ProdCats!C112&amp;"],"</f>
+        <v>['product_id'=&gt;72,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A113&amp;",'category_id'=&gt;"&amp;ProdCats!C113&amp;"],"</f>
+        <v>['product_id'=&gt;107,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A114&amp;",'category_id'=&gt;"&amp;ProdCats!C114&amp;"],"</f>
+        <v>['product_id'=&gt;108,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A115&amp;",'category_id'=&gt;"&amp;ProdCats!C115&amp;"],"</f>
+        <v>['product_id'=&gt;109,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A116&amp;",'category_id'=&gt;"&amp;ProdCats!C116&amp;"],"</f>
+        <v>['product_id'=&gt;110,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A117&amp;",'category_id'=&gt;"&amp;ProdCats!C117&amp;"],"</f>
+        <v>['product_id'=&gt;111,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A118&amp;",'category_id'=&gt;"&amp;ProdCats!C118&amp;"],"</f>
+        <v>['product_id'=&gt;112,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A119&amp;",'category_id'=&gt;"&amp;ProdCats!C119&amp;"],"</f>
+        <v>['product_id'=&gt;113,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A120&amp;",'category_id'=&gt;"&amp;ProdCats!C120&amp;"],"</f>
+        <v>['product_id'=&gt;114,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A121&amp;",'category_id'=&gt;"&amp;ProdCats!C121&amp;"],"</f>
+        <v>['product_id'=&gt;115,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A122&amp;",'category_id'=&gt;"&amp;ProdCats!C122&amp;"],"</f>
+        <v>['product_id'=&gt;116,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A123&amp;",'category_id'=&gt;"&amp;ProdCats!C123&amp;"],"</f>
+        <v>['product_id'=&gt;117,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A124&amp;",'category_id'=&gt;"&amp;ProdCats!C124&amp;"],"</f>
+        <v>['product_id'=&gt;118,'category_id'=&gt;17],</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A125&amp;",'category_id'=&gt;"&amp;ProdCats!C125&amp;"],"</f>
+        <v>['product_id'=&gt;76,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A126&amp;",'category_id'=&gt;"&amp;ProdCats!C126&amp;"],"</f>
+        <v>['product_id'=&gt;77,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A127&amp;",'category_id'=&gt;"&amp;ProdCats!C127&amp;"],"</f>
+        <v>['product_id'=&gt;78,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A128&amp;",'category_id'=&gt;"&amp;ProdCats!C128&amp;"],"</f>
+        <v>['product_id'=&gt;119,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A129&amp;",'category_id'=&gt;"&amp;ProdCats!C129&amp;"],"</f>
+        <v>['product_id'=&gt;120,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A130&amp;",'category_id'=&gt;"&amp;ProdCats!C130&amp;"],"</f>
+        <v>['product_id'=&gt;121,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A131&amp;",'category_id'=&gt;"&amp;ProdCats!C131&amp;"],"</f>
+        <v>['product_id'=&gt;122,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A132&amp;",'category_id'=&gt;"&amp;ProdCats!C132&amp;"],"</f>
+        <v>['product_id'=&gt;123,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A133&amp;",'category_id'=&gt;"&amp;ProdCats!C133&amp;"],"</f>
+        <v>['product_id'=&gt;124,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A134&amp;",'category_id'=&gt;"&amp;ProdCats!C134&amp;"],"</f>
+        <v>['product_id'=&gt;125,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A135&amp;",'category_id'=&gt;"&amp;ProdCats!C135&amp;"],"</f>
+        <v>['product_id'=&gt;126,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A136&amp;",'category_id'=&gt;"&amp;ProdCats!C136&amp;"],"</f>
+        <v>['product_id'=&gt;127,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A137&amp;",'category_id'=&gt;"&amp;ProdCats!C137&amp;"],"</f>
+        <v>['product_id'=&gt;128,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A138&amp;",'category_id'=&gt;"&amp;ProdCats!C138&amp;"],"</f>
+        <v>['product_id'=&gt;129,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A139&amp;",'category_id'=&gt;"&amp;ProdCats!C139&amp;"],"</f>
+        <v>['product_id'=&gt;130,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A140&amp;",'category_id'=&gt;"&amp;ProdCats!C140&amp;"],"</f>
+        <v>['product_id'=&gt;112,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A141&amp;",'category_id'=&gt;"&amp;ProdCats!C141&amp;"],"</f>
+        <v>['product_id'=&gt;131,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A142&amp;",'category_id'=&gt;"&amp;ProdCats!C142&amp;"],"</f>
+        <v>['product_id'=&gt;132,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A143&amp;",'category_id'=&gt;"&amp;ProdCats!C143&amp;"],"</f>
+        <v>['product_id'=&gt;113,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A144&amp;",'category_id'=&gt;"&amp;ProdCats!C144&amp;"],"</f>
+        <v>['product_id'=&gt;133,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A145&amp;",'category_id'=&gt;"&amp;ProdCats!C145&amp;"],"</f>
+        <v>['product_id'=&gt;134,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A146&amp;",'category_id'=&gt;"&amp;ProdCats!C146&amp;"],"</f>
+        <v>['product_id'=&gt;135,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A147&amp;",'category_id'=&gt;"&amp;ProdCats!C147&amp;"],"</f>
+        <v>['product_id'=&gt;114,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A148&amp;",'category_id'=&gt;"&amp;ProdCats!C148&amp;"],"</f>
+        <v>['product_id'=&gt;136,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A149&amp;",'category_id'=&gt;"&amp;ProdCats!C149&amp;"],"</f>
+        <v>['product_id'=&gt;137,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A150&amp;",'category_id'=&gt;"&amp;ProdCats!C150&amp;"],"</f>
+        <v>['product_id'=&gt;138,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A151&amp;",'category_id'=&gt;"&amp;ProdCats!C151&amp;"],"</f>
+        <v>['product_id'=&gt;139,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A152&amp;",'category_id'=&gt;"&amp;ProdCats!C152&amp;"],"</f>
+        <v>['product_id'=&gt;140,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A153&amp;",'category_id'=&gt;"&amp;ProdCats!C153&amp;"],"</f>
+        <v>['product_id'=&gt;141,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A154&amp;",'category_id'=&gt;"&amp;ProdCats!C154&amp;"],"</f>
+        <v>['product_id'=&gt;142,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A155&amp;",'category_id'=&gt;"&amp;ProdCats!C155&amp;"],"</f>
+        <v>['product_id'=&gt;143,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A156&amp;",'category_id'=&gt;"&amp;ProdCats!C156&amp;"],"</f>
+        <v>['product_id'=&gt;144,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A157&amp;",'category_id'=&gt;"&amp;ProdCats!C157&amp;"],"</f>
+        <v>['product_id'=&gt;145,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A158&amp;",'category_id'=&gt;"&amp;ProdCats!C158&amp;"],"</f>
+        <v>['product_id'=&gt;146,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A159&amp;",'category_id'=&gt;"&amp;ProdCats!C159&amp;"],"</f>
+        <v>['product_id'=&gt;147,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A160&amp;",'category_id'=&gt;"&amp;ProdCats!C160&amp;"],"</f>
+        <v>['product_id'=&gt;148,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A161&amp;",'category_id'=&gt;"&amp;ProdCats!C161&amp;"],"</f>
+        <v>['product_id'=&gt;149,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A162&amp;",'category_id'=&gt;"&amp;ProdCats!C162&amp;"],"</f>
+        <v>['product_id'=&gt;150,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A163&amp;",'category_id'=&gt;"&amp;ProdCats!C163&amp;"],"</f>
+        <v>['product_id'=&gt;151,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A164&amp;",'category_id'=&gt;"&amp;ProdCats!C164&amp;"],"</f>
+        <v>['product_id'=&gt;152,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A165&amp;",'category_id'=&gt;"&amp;ProdCats!C165&amp;"],"</f>
+        <v>['product_id'=&gt;153,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A166&amp;",'category_id'=&gt;"&amp;ProdCats!C166&amp;"],"</f>
+        <v>['product_id'=&gt;154,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A167&amp;",'category_id'=&gt;"&amp;ProdCats!C167&amp;"],"</f>
+        <v>['product_id'=&gt;155,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A168&amp;",'category_id'=&gt;"&amp;ProdCats!C168&amp;"],"</f>
+        <v>['product_id'=&gt;156,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A169&amp;",'category_id'=&gt;"&amp;ProdCats!C169&amp;"],"</f>
+        <v>['product_id'=&gt;157,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A170&amp;",'category_id'=&gt;"&amp;ProdCats!C170&amp;"],"</f>
+        <v>['product_id'=&gt;158,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A171&amp;",'category_id'=&gt;"&amp;ProdCats!C171&amp;"],"</f>
+        <v>['product_id'=&gt;159,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="str">
+        <f>"['product_id'=&gt;"&amp;ProdCats!A172&amp;",'category_id'=&gt;"&amp;ProdCats!C172&amp;"],"</f>
+        <v>['product_id'=&gt;160,'category_id'=&gt;18],</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed level column value
</commit_message>
<xml_diff>
--- a/docs/Products.xlsx
+++ b/docs/Products.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Prds" sheetId="2" r:id="rId1"/>
@@ -4195,7 +4195,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4292,7 +4292,7 @@
         <v>200</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
@@ -4571,7 +4571,7 @@
         <v>201</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
         <v>34</v>
@@ -10949,7 +10949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
@@ -10964,7 +10964,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>"['id'=&gt;"&amp;Cats!A4&amp;",'name'=&gt;'"&amp;Cats!B4&amp;"','slug'=&gt;'"&amp;Cats!C4&amp;"','parent_id'=&gt;"&amp;Cats!E4&amp;",'type'=&gt;'"&amp;Cats!F4&amp;"','ord'=&gt;"&amp;Cats!G4&amp;",'lvl'=&gt;"&amp;Cats!H4&amp;",'description'=&gt;'"&amp;Cats!I4&amp;"'],"</f>
-        <v>['id'=&gt;2,'name'=&gt;'Speakers','slug'=&gt;'speakers','parent_id'=&gt;NULL,'type'=&gt;'group','ord'=&gt;200,'lvl'=&gt;1,'description'=&gt;'Powerful performance. Versatile designs. For all your music, movies, and tv — at home or on the go.'],</v>
+        <v>['id'=&gt;2,'name'=&gt;'Speakers','slug'=&gt;'speakers','parent_id'=&gt;NULL,'type'=&gt;'group','ord'=&gt;200,'lvl'=&gt;0,'description'=&gt;'Powerful performance. Versatile designs. For all your music, movies, and tv — at home or on the go.'],</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -11018,7 +11018,7 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>"['id'=&gt;"&amp;Cats!A13&amp;",'name'=&gt;'"&amp;Cats!B13&amp;"','slug'=&gt;'"&amp;Cats!C13&amp;"','parent_id'=&gt;"&amp;Cats!E13&amp;",'type'=&gt;'"&amp;Cats!F13&amp;"','ord'=&gt;"&amp;Cats!G13&amp;",'lvl'=&gt;"&amp;Cats!H13&amp;",'description'=&gt;'"&amp;Cats!I13&amp;"'],"</f>
-        <v>['id'=&gt;11,'name'=&gt;'Portable','slug'=&gt;'portable','parent_id'=&gt;2,'type'=&gt;'product','ord'=&gt;201,'lvl'=&gt;0,'description'=&gt;'Engineered to travel, but sound great in your home. With durable designs and impressive battery life, you can bring them wherever music takes you.'],</v>
+        <v>['id'=&gt;11,'name'=&gt;'Portable','slug'=&gt;'portable','parent_id'=&gt;2,'type'=&gt;'product','ord'=&gt;201,'lvl'=&gt;1,'description'=&gt;'Engineered to travel, but sound great in your home. With durable designs and impressive battery life, you can bring them wherever music takes you.'],</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -11072,7 +11072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>